<commit_message>
added R preprocessing script for downloading APRA banking stats and consolidating latest states with back series
added js app for viewing data online
</commit_message>
<xml_diff>
--- a/Data/APRA Reporting Institute Names by Sector.xlsx
+++ b/Data/APRA Reporting Institute Names by Sector.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kadre\Kadre\APRA\gitaprarepo\Apra-Monthly-Deposits\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cklettner/Kadre/Apra-Monthly-Deposits/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D9215F-5E86-482C-A958-8088B6080793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBC9F8B-2AEC-BF41-9075-8603E0856A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14280" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="SectorNames" sheetId="2" r:id="rId2"/>
+    <sheet name="ColNames" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="225">
   <si>
     <t>Institute_Name</t>
   </si>
@@ -77,9 +78,6 @@
     <t>Australian Settlements Limited</t>
   </si>
   <si>
-    <t>Mtuals/Customer Owned</t>
-  </si>
-  <si>
     <t>Australian Unity Bank Limited</t>
   </si>
   <si>
@@ -173,9 +171,6 @@
     <t>Credit Suisse AG</t>
   </si>
   <si>
-    <t>Internation Investment</t>
-  </si>
-  <si>
     <t>Credit Union Australia Ltd</t>
   </si>
   <si>
@@ -500,15 +495,6 @@
     <t>Sector names</t>
   </si>
   <si>
-    <t>RACQ</t>
-  </si>
-  <si>
-    <t>Challenger</t>
-  </si>
-  <si>
-    <t>the hong</t>
-  </si>
-  <si>
     <t>Challenger Bank Limited</t>
   </si>
   <si>
@@ -518,7 +504,199 @@
     <t>NongHyup Bank</t>
   </si>
   <si>
-    <t>Societe  Generale</t>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>ABN</t>
+  </si>
+  <si>
+    <t>Institution Name</t>
+  </si>
+  <si>
+    <t>Cash and liquid assets</t>
+  </si>
+  <si>
+    <t>Cash and deposits with financial institutions</t>
+  </si>
+  <si>
+    <t>Trading securities</t>
+  </si>
+  <si>
+    <t>Investment securities</t>
+  </si>
+  <si>
+    <t>Acceptances of customers</t>
+  </si>
+  <si>
+    <t>Net acceptances of customers</t>
+  </si>
+  <si>
+    <t>Gross loans and advances</t>
+  </si>
+  <si>
+    <t>Drop1</t>
+  </si>
+  <si>
+    <t>Other investments</t>
+  </si>
+  <si>
+    <t>Drop2</t>
+  </si>
+  <si>
+    <t>Total resident assets</t>
+  </si>
+  <si>
+    <t>Total residents assets</t>
+  </si>
+  <si>
+    <t>Outstanding value of all assets that have been securitised</t>
+  </si>
+  <si>
+    <t>Total securitised assets on balance sheet</t>
+  </si>
+  <si>
+    <t>Outstanding principal balance of securitised assets</t>
+  </si>
+  <si>
+    <t>Drop3</t>
+  </si>
+  <si>
+    <t>Value of housing loans securitised</t>
+  </si>
+  <si>
+    <t>Drop4</t>
+  </si>
+  <si>
+    <t>Value of housing loans securitised during the month</t>
+  </si>
+  <si>
+    <t>Drop5</t>
+  </si>
+  <si>
+    <t>Loans to non-financial corporations</t>
+  </si>
+  <si>
+    <t>Loans to non-financial businesses</t>
+  </si>
+  <si>
+    <t>Loans to financial corporations</t>
+  </si>
+  <si>
+    <t>Loans to financial institutions</t>
+  </si>
+  <si>
+    <t>Loans to general government</t>
+  </si>
+  <si>
+    <t>Loans to households: Housing: Owner-occupied</t>
+  </si>
+  <si>
+    <t>Loans to households: Housing: Investment</t>
+  </si>
+  <si>
+    <t>Loans to households: Credit cards</t>
+  </si>
+  <si>
+    <t>Loans to households: Other</t>
+  </si>
+  <si>
+    <t>Loans to community service organisations and non-profit institutions</t>
+  </si>
+  <si>
+    <t>Loans to community service organisations</t>
+  </si>
+  <si>
+    <t>Total gross loans and advances</t>
+  </si>
+  <si>
+    <t>Total residents loans and finance leases</t>
+  </si>
+  <si>
+    <t>Intra-group loans and advances</t>
+  </si>
+  <si>
+    <t>Intra-group loans and finance leases</t>
+  </si>
+  <si>
+    <t>Due to clearing houses and financial institutions</t>
+  </si>
+  <si>
+    <t>Drop6</t>
+  </si>
+  <si>
+    <t>Acceptances</t>
+  </si>
+  <si>
+    <t>Total deposits</t>
+  </si>
+  <si>
+    <t>Drop7</t>
+  </si>
+  <si>
+    <t>Intra-group deposits</t>
+  </si>
+  <si>
+    <t>Bonds, notes and long-term borrowings</t>
+  </si>
+  <si>
+    <t>Total long-term borrowings</t>
+  </si>
+  <si>
+    <t>Other borrowings</t>
+  </si>
+  <si>
+    <t>Total short-term borrowings</t>
+  </si>
+  <si>
+    <t>Deposits from non-financial corporations</t>
+  </si>
+  <si>
+    <t>Deposits by non-financial businesses</t>
+  </si>
+  <si>
+    <t>Deposits from financial corporations</t>
+  </si>
+  <si>
+    <t>Deposits by financial institutions</t>
+  </si>
+  <si>
+    <t>Deposits from general government</t>
+  </si>
+  <si>
+    <t>Deposits by general government</t>
+  </si>
+  <si>
+    <t>Deposits from households</t>
+  </si>
+  <si>
+    <t>Deposits by households</t>
+  </si>
+  <si>
+    <t>Deposits from community service organisations and non-profit institutions</t>
+  </si>
+  <si>
+    <t>Deposits by community service organisations</t>
+  </si>
+  <si>
+    <t>Other deposit accounts</t>
+  </si>
+  <si>
+    <t>Drop8</t>
+  </si>
+  <si>
+    <t>Certificates of deposit</t>
+  </si>
+  <si>
+    <t>Negotiable Certificates of Deposit</t>
+  </si>
+  <si>
+    <t>Total residents deposits</t>
   </si>
 </sst>
 </file>
@@ -536,31 +714,34 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -625,10 +806,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -847,21 +1028,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="C146" sqref="C146"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -872,9 +1052,8 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -885,9 +1064,8 @@
         <v>4</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -898,9 +1076,8 @@
         <v>4</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -911,9 +1088,8 @@
         <v>7</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -924,9 +1100,8 @@
         <v>9</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -939,9 +1114,8 @@
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -952,9 +1126,8 @@
         <v>14</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -965,9 +1138,8 @@
         <v>14</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -978,9 +1150,8 @@
         <v>14</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -988,355 +1159,328 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>11</v>
@@ -1344,473 +1488,437 @@
       <c r="D37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>48</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>50</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <v>56</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>58</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>59</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>61</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>62</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>63</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
         <v>64</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
         <v>65</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
         <v>66</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>67</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
         <v>68</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>69</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>7</v>
@@ -1818,109 +1926,97 @@
       <c r="D73" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>72</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-    </row>
-    <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
         <v>73</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-    </row>
-    <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <v>74</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D76" s="1"/>
-      <c r="E76" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
         <v>75</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-    </row>
-    <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-    </row>
-    <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
         <v>77</v>
       </c>
-      <c r="B79" s="7" t="s">
-        <v>91</v>
+      <c r="B79" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>11</v>
@@ -1928,586 +2024,541 @@
       <c r="D81" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
         <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-    </row>
-    <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
         <v>83</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-    </row>
-    <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-    </row>
-    <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-    </row>
-    <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-    </row>
-    <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
         <v>90</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="5">
         <v>91</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>92</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-    </row>
-    <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <v>93</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-    </row>
-    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <v>94</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-    </row>
-    <row r="97" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>95</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-    </row>
-    <row r="98" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="5">
         <v>96</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-    </row>
-    <row r="99" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="5">
         <v>97</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-    </row>
-    <row r="100" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-    </row>
-    <row r="101" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="5">
         <v>99</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-    </row>
-    <row r="102" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="5">
         <v>100</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-    </row>
-    <row r="103" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="5">
         <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D103" s="1"/>
-      <c r="E103" s="1"/>
-    </row>
-    <row r="104" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="5">
         <v>102</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-    </row>
-    <row r="105" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="5">
         <v>103</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-    </row>
-    <row r="106" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="5">
         <v>104</v>
       </c>
-      <c r="B106" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C106" s="7" t="s">
+      <c r="B106" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C106" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-    </row>
-    <row r="107" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>105</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-    </row>
-    <row r="108" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <v>106</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-    </row>
-    <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>107</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-    </row>
-    <row r="110" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="5">
         <v>108</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-    </row>
-    <row r="111" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="5">
         <v>109</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
-    </row>
-    <row r="112" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="5">
         <v>110</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-    </row>
-    <row r="113" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A113" s="5">
         <v>111</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
-    </row>
-    <row r="114" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A114" s="5">
         <v>112</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-    </row>
-    <row r="115" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A115" s="5">
         <v>113</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-    </row>
-    <row r="116" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A116" s="5">
         <v>114</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-    </row>
-    <row r="117" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>115</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
-    </row>
-    <row r="118" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A118" s="5">
         <v>116</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-    </row>
-    <row r="119" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A119" s="5">
         <v>117</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
-    </row>
-    <row r="120" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A120" s="5">
         <v>118</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
-    </row>
-    <row r="121" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A121" s="5">
         <v>119</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-    </row>
-    <row r="122" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A122" s="5">
         <v>120</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-    </row>
-    <row r="123" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A123" s="5">
         <v>121</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
-    </row>
-    <row r="124" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A124" s="5">
         <v>122</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
-    </row>
-    <row r="125" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A125" s="5">
         <v>123</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-    </row>
-    <row r="126" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" s="5">
         <v>124</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>11</v>
@@ -2515,313 +2566,267 @@
       <c r="D126" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E126" s="1"/>
-    </row>
-    <row r="127" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A127" s="5">
         <v>125</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
-    </row>
-    <row r="128" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A128" s="5">
         <v>126</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C128" s="7" t="s">
-        <v>44</v>
+        <v>138</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
-    </row>
-    <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A129" s="5">
         <v>127</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
-    </row>
-    <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A130" s="5">
         <v>128</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
-    </row>
-    <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A131" s="5">
         <v>129</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D131" s="1"/>
-      <c r="E131" s="1"/>
-    </row>
-    <row r="132" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A132" s="5">
         <v>130</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D132" s="1"/>
-      <c r="E132" s="1"/>
-    </row>
-    <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A133" s="5">
         <v>131</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D133" s="1"/>
-      <c r="E133" s="1"/>
-    </row>
-    <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A134" s="5">
         <v>132</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D134" s="1"/>
-      <c r="E134" s="1"/>
-    </row>
-    <row r="135" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A135" s="5">
         <v>133</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D135" s="1"/>
-      <c r="E135" s="1"/>
-    </row>
-    <row r="136" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A136" s="5">
         <v>134</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D136" s="1"/>
+    </row>
+    <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A137" s="5">
+        <v>136</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="1"/>
+    </row>
+    <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A138" s="5">
+        <v>137</v>
+      </c>
+      <c r="B138" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C136" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D136" s="1"/>
-      <c r="E136" s="1"/>
-    </row>
-    <row r="137" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A137" s="5">
-        <v>135</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D137" s="1"/>
-      <c r="E137" s="1"/>
-    </row>
-    <row r="138" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A138" s="5">
-        <v>136</v>
-      </c>
-      <c r="B138" s="1" t="s">
+      <c r="C138" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D138" s="1"/>
+    </row>
+    <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A139" s="5">
+        <v>138</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C138" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D138" s="1"/>
-      <c r="E138" s="1"/>
-    </row>
-    <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A139" s="5">
-        <v>137</v>
-      </c>
-      <c r="B139" s="1" t="s">
+      <c r="C139" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D139" s="1"/>
+    </row>
+    <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A140" s="5">
+        <v>139</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C139" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D139" s="1"/>
-      <c r="E139" s="1"/>
-    </row>
-    <row r="140" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A140" s="5">
-        <v>138</v>
-      </c>
-      <c r="B140" s="1" t="s">
+      <c r="C140" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D140" s="1"/>
+    </row>
+    <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A141" s="5">
+        <v>140</v>
+      </c>
+      <c r="B141" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C140" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D140" s="1"/>
-      <c r="E140" s="1"/>
-    </row>
-    <row r="141" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A141" s="5">
-        <v>139</v>
-      </c>
-      <c r="B141" s="1" t="s">
+      <c r="C141" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141" s="1"/>
+    </row>
+    <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A142" s="5">
+        <v>141</v>
+      </c>
+      <c r="B142" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C141" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D141" s="1"/>
-      <c r="E141" s="1"/>
-    </row>
-    <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A142" s="5">
-        <v>140</v>
-      </c>
-      <c r="B142" s="1" t="s">
+      <c r="C142" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D142" s="1"/>
+    </row>
+    <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A143" s="5">
+        <v>142</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D142" s="1"/>
-      <c r="E142" s="1"/>
-    </row>
-    <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A143" s="5">
-        <v>141</v>
-      </c>
-      <c r="B143" s="1" t="s">
+      <c r="C143" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" s="1"/>
+    </row>
+    <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A144" s="5">
+        <v>143</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C143" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D143" s="1"/>
-      <c r="E143" s="1"/>
-    </row>
-    <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A144" s="5">
-        <v>142</v>
-      </c>
-      <c r="B144" s="1" t="s">
+      <c r="C144" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" s="1"/>
+    </row>
+    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A145" s="5">
+        <v>144</v>
+      </c>
+      <c r="B145" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C144" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D144" s="1"/>
-      <c r="E144" s="1"/>
-    </row>
-    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A145" s="5">
-        <v>143</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="C145" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D145" s="1"/>
-      <c r="E145" s="1"/>
-    </row>
-    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A146" s="5">
-        <v>144</v>
-      </c>
-      <c r="B146" s="1" t="s">
+    </row>
+    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>145</v>
+      </c>
+      <c r="B146" t="s">
         <v>157</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="D146" s="1"/>
-      <c r="E146" s="1"/>
-    </row>
-    <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="D147" s="1"/>
-      <c r="E147" s="1"/>
-    </row>
-    <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A148" s="1">
-        <v>146</v>
+    </row>
+    <row r="148" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="7">
+        <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D148" s="1"/>
-      <c r="E148" s="1"/>
-    </row>
-    <row r="149" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="8">
-        <v>147</v>
-      </c>
-      <c r="B149" t="s">
-        <v>164</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="8">
-        <v>148</v>
-      </c>
-      <c r="B150" t="s">
-        <v>165</v>
-      </c>
-      <c r="C150" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2838,53 +2843,387 @@
   </sheetPr>
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAD3895F-F975-9F46-A533-D754E4C99139}">
+  <dimension ref="A1:C39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="54.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>205</v>
+      </c>
+      <c r="B29" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>206</v>
+      </c>
+      <c r="B30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B31" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>210</v>
+      </c>
+      <c r="B32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>212</v>
+      </c>
+      <c r="B33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>214</v>
+      </c>
+      <c r="B34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>218</v>
+      </c>
+      <c r="B36" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>222</v>
+      </c>
+      <c r="B38" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>